<commit_message>
Aggiunto metodo per scegliere dove savare il file
</commit_message>
<xml_diff>
--- a/Partecipanti.xlsx
+++ b/Partecipanti.xlsx
@@ -10,10 +10,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -377,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -401,53 +399,53 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve">Bollea </v>
+        <v xml:space="preserve">Aimaro </v>
       </c>
       <c r="B2" t="str">
-        <v>Ivan</v>
+        <v>Roberto</v>
       </c>
       <c r="C2" t="str">
-        <v>17/7/1975</v>
+        <v>10/9/1965</v>
       </c>
       <c r="D2" t="str">
-        <v>BLLVNI75L17L750M</v>
+        <v>MRARRT65P10L219N</v>
       </c>
       <c r="E2" t="str">
-        <v>Cigliano</v>
+        <v>cig</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Capra</v>
+        <v>Bobba</v>
       </c>
       <c r="B3" t="str">
-        <v>Franco</v>
+        <v>Adriano</v>
       </c>
       <c r="C3" t="str">
-        <v>23/11/1955</v>
+        <v>16/8/1960</v>
       </c>
       <c r="D3" t="str">
-        <v>CPRFNC55S23C680Q</v>
+        <v>BBBDRN60M16H725J</v>
       </c>
       <c r="E3" t="str">
-        <v>Cigliano</v>
+        <v>cig</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Giolito</v>
+        <v xml:space="preserve">Bollea </v>
       </c>
       <c r="B4" t="str">
-        <v>Giovanni</v>
+        <v>Alberto</v>
       </c>
       <c r="C4" t="str">
-        <v>25/10/1959</v>
+        <v>13/11/2012</v>
       </c>
       <c r="D4" t="str">
-        <v>GLTGNN59R25C680U</v>
+        <v>BLLLRT12S13L219J</v>
       </c>
       <c r="E4" t="str">
-        <v>Cigliano</v>
+        <v>cig</v>
       </c>
     </row>
     <row r="5">
@@ -464,63 +462,29 @@
         <v>PPVNKL93R02Z149L</v>
       </c>
       <c r="E5" t="str">
-        <v>Cigliano</v>
+        <v>cig</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v xml:space="preserve">Grippo </v>
+        <v>Regis</v>
       </c>
       <c r="B6" t="str">
-        <v>Sandro</v>
+        <v>Maurizio</v>
       </c>
       <c r="C6" t="str">
-        <v>17/6/1978</v>
+        <v>7/2/1974</v>
       </c>
       <c r="D6" t="str">
-        <v>GRPSDR78H17H703M</v>
+        <v>RGSMRZ74B07C665P</v>
       </c>
       <c r="E6" t="str">
-        <v>Livorno</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Invernizzi</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Attilio</v>
-      </c>
-      <c r="C7" t="str">
-        <v>12/11/1950</v>
-      </c>
-      <c r="D7" t="str">
-        <v>NVRTTL50S12C680U</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Livorno</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Notarrigo</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Vincenzo</v>
-      </c>
-      <c r="C8" t="str">
-        <v>31/12/1975</v>
-      </c>
-      <c r="D8" t="str">
-        <v>NTRVCN75T31C342N</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Livorno</v>
+        <v>cig</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>